<commit_message>
Added 2 Error Handling
</commit_message>
<xml_diff>
--- a/InAuto_Project_2200589F_2202465G/InternshipEmails.xlsx
+++ b/InAuto_Project_2200589F_2202465G/InternshipEmails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78df99500250e0aa/Documents/GitHub/InAuto/InAuto_Project_2200589F_2202465G/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="8_{C36450E1-70C5-4284-8724-A0A78D84726F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{112F84F3-7689-46A9-B419-EAFAC057462A}"/>
+  <xr:revisionPtr revIDLastSave="198" documentId="8_{C36450E1-70C5-4284-8724-A0A78D84726F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4460674-0E73-4984-84EB-7E0BD29A0DD9}"/>
   <bookViews>
     <workbookView xWindow="5220" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{A8753D73-CDB8-4E0C-8DDE-BB08DD8360D8}"/>
   </bookViews>
@@ -41,87 +41,89 @@
     <t>Email Applications</t>
   </si>
   <si>
-    <t>Subject: Application for Front-End Developer Internship Position_x000D_
+    <t>Subject: Application for Front-End Developer/Software Intern Position at Aevice Health_x000D_
 _x000D_
 Dear Hiring Manager,_x000D_
 _x000D_
-I am writing to express my interest in the Front-End Developer Internship position at Aevice Health, as discovered on Glints.com. As a second-year student pursuing a Diploma in Computer Engineering at Temasek Polytechnic, I am deeply motivated to learn from experienced engineers and continue my journey in software development, inspired by my father's legacy in engineering._x000D_
-_x000D_
-With a solid foundation in Python, Java, and C, I have honed my technical skills through various projects. In Python, I've utilized libraries like NumPy and Matplotlib for enhanced data visualization. My experience in Java includes developing systems following the MVC pattern, emphasizing CRUD operations and user management. Additionally, I've worked on embedded systems in C, focusing on hardware-software integration. These experiences have equipped me with a strong understanding of software development principles and practices._x000D_
-_x000D_
-Beyond technical proficiency, I bring a range of soft skills essential for collaborative environments. I excel in teamwork, leveraging active listening and effective communication to ensure project success. My critical thinking abilities enable me to analyze problems and make informed decisions, ensuring tasks are completed accurately and efficiently. I am eager to apply these skills within a dynamic team environment at Aevice Health._x000D_
-_x000D_
-I am excited about the opportunity to contribute to Aevice Health's mission of revolutionizing healthcare through innovative technology. The prospect of working in a fast-paced startup environment, alongside passionate professionals, aligns perfectly with my career aspirations. I am confident that my technical expertise and interpersonal skills make me a valuable addition to your team._x000D_
-_x000D_
-Thank you for considering my application. I look forward to the possibility of discussing how I can contribute to Aevice Health's success. _x000D_
+I am writing to express my interest in the Front-End Developer/Software Intern position at Aevice Health, as advertised on Glints.com. My name is Chuang Kai Siang, currently pursuing a Diploma in Computer Engineering at Temasek Polytechnic in my second year. I discovered this opportunity through Glints.com and was immediately drawn to Aevice Health due to its innovative approach to improving the lives of patients with chronic respiratory diseases, a cause close to my heart. Moreover, I am motivated to apply for this role as it aligns with my strong desire to learn from experienced engineers and follow in my father's footsteps, who holds a master's degree in engineering._x000D_
+_x000D_
+In terms of technical skills, I bring a robust foundation in programming languages such as Python, Java, and C. In Python, I have experience leveraging libraries like NumPy and Matplotlib for enhanced data visualization. My proficiency in Java extends to developing systems following the MVC pattern, implementing CRUD operations, and managing user interactions. Additionally, my expertise in C includes designing and integrating hardware and software for embedded systems. These technical skills position me well to contribute effectively to the development, testing, and maintenance of mobile and web applications at Aevice Health._x000D_
+_x000D_
+Complementing my technical abilities are my soft skills, which include a collaborative approach to teamwork, effective communication, and critical problem-solving. I excel in actively listening to team members' perspectives and offering valuable insights to drive project success. My ability to think critically and analytically ensures tasks are completed with precision and accuracy, contributing to a seamless development process. I am eager to further cultivate these skills within the dynamic environment at Aevice Health, where innovation and creativity are celebrated._x000D_
+_x000D_
+I am available for the flexible start/end dates specified in the job description and have included my GitHub profile in my application for your reference. I am excited about the opportunity to contribute to Aevice Health's mission and eager to gain hands-on experience in the software development lifecycle. Thank you for considering my application. _x000D_
 _x000D_
 Best Regards,_x000D_
 Chuang Kai Siang</t>
   </si>
   <si>
-    <t>Subject: Application for Frontend Web Developer Position at El Pando Pte Ltd_x000D_
+    <t>Subject: Application for Software Engineer - Remote Position_x000D_
 _x000D_
 Dear Hiring Manager,_x000D_
 _x000D_
-I am writing to express my interest in the Frontend Web Developer position at El Pando Pte Ltd, which I discovered through Glints.com. My name is Chuang Kai Siang, currently pursuing a Diploma in Computer Engineering at Temasek Polytechnic in my second year. I am drawn to this opportunity due to my strong desire to learn from experienced engineers, inspired by my father who holds a master's in engineering, and contribute to impactful projects in a dynamic environment._x000D_
-_x000D_
-With a solid foundation in technical skills, I have experience in Python for data visualization, Java for system development following MVC architecture, and C for embedded systems design and integration. These skills have equipped me with a problem-solving mindset and a knack for collaborative teamwork. Moreover, my proactive approach and strong communication skills enable me to effectively engage with team members and stakeholders, ensuring tasks are completed accurately and efficiently._x000D_
-_x000D_
-In addition to my technical proficiency, I bring a passion for design and a curiosity for emerging web trends, aligning with the role's emphasis on frontend development and staying abreast of industry innovations. I am eager to contribute my skills to El Pando's noteworthy projects, collaborate with experienced developers, and embrace the vibrant culture of continuous learning and growth._x000D_
-_x000D_
-Thank you for considering my application. I am enthusiastic about the opportunity to further discuss how my background, skills, and motivations align with the needs of El Pando Pte Ltd. _x000D_
+I hope this email finds you well. My name is Chuang Kai Siang, and I am writing to express my interest in the Software Engineer position at Kopi Date, as advertised on Glints.com. As a second-year student pursuing a Diploma in Computer Engineering at Temasek Polytechnic, I am deeply motivated to learn from experienced engineers and continue the legacy set by my father, who holds a master's degree in engineering._x000D_
+_x000D_
+My journey into the world of programming began with Python, where I gained proficiency in utilizing libraries such as NumPy and Matplotlib for advanced data visualization. Additionally, my experience with Java involved developing systems following the MVC pattern, focusing on CRUD operations and user management. Furthermore, I have a solid foundation in C, particularly in implementing embedded systems that integrate hardware and software seamlessly._x000D_
+_x000D_
+Beyond technical expertise, I bring a set of soft skills that complement my technical capabilities. I excel in collaborative teamwork, leveraging strong active listening and interpersonal communication skills to foster a cohesive work environment. My ability to think critically and analytically enables me to solve problems effectively, ensuring tasks are completed with precision and accuracy._x000D_
+_x000D_
+I am particularly drawn to Kopi Date's commitment to developing user features, optimizing operations, and enhancing machine learning algorithms. My skills in JavaScript, Node.js, and Firebase align well with the role's requirements, and I am eager to contribute to the development of innovative solutions while continuously learning and growing within your dynamic team._x000D_
+_x000D_
+Thank you for considering my application. I am enthusiastic about the opportunity to further discuss how my skills and experiences align with the needs of Kopi Date. Please find my attached resume for more details. _x000D_
 _x000D_
 Best Regards,_x000D_
 Chuang Kai Siang</t>
   </si>
   <si>
-    <t>Subject: Application for Network &amp; Systems Engineer Position_x000D_
+    <t>Subject: Application for Junior Software Developer Position at Mavericks Consulting_x000D_
 _x000D_
 Dear Hiring Manager,_x000D_
 _x000D_
-I hope this email finds you well. My name is Chuang Kai Siang, and I recently came across the Network &amp; Systems Engineer position at eVantage Technology Pte Ltd through Glints.com. With a strong desire to learn from experienced engineers and inspired by my father's engineering background, I am excited to apply for this role._x000D_
-_x000D_
-In my second year pursuing a Diploma in Computer Engineering at Temasek Polytechnic, I have honed my technical skills through hands-on experience and academic coursework. Proficient in Python, Java, and C, I have developed systems implementing CRUD operations, user management, and embedded systems integration. Moreover, my ability to leverage Python libraries like NumPy and Matplotlib for data visualization enhances my problem-solving capabilities._x000D_
-_x000D_
-Complementing my technical expertise, I possess exceptional soft skills essential for effective collaboration and communication in team environments. Skilled in active listening and interpersonal communication, I excel in collaborative teamwork, ensuring tasks are completed accurately and efficiently. Moreover, my critical thinking abilities enable me to analyze problems systematically and make informed decisions to achieve optimal outcomes._x000D_
-_x000D_
-With a keen interest in IT solutions and a track record of academic excellence and practical application, I am confident in my ability to contribute effectively to eVantage Technology's engineering team. I am eager to leverage my skills to provide quality support to clients, participate in project planning and implementation, and contribute to the success of your organization._x000D_
-_x000D_
-Thank you for considering my application. I am looking forward to the opportunity to further discuss how my skills and experiences align with the needs of eVantage Technology Pte Ltd. _x000D_
+I hope this email finds you well. I am writing to express my keen interest in the Junior Software Developer position at Mavericks Consulting, as advertised on Glints.com. My name is Chuang Kai Siang, currently pursuing a Diploma in Computer Engineering at Temasek Polytechnic, Singapore, in my second year._x000D_
+_x000D_
+My journey into the world of software development has been inspired by my father, who holds a master's degree in engineering. I am eager to follow in his footsteps and learn from experienced engineers like those at Mavericks Consulting. My main motivation for applying is to immerse myself in a dynamic environment where I can continuously grow and contribute to meaningful projects._x000D_
+_x000D_
+With a solid foundation in technical skills, I have hands-on experience in Python, utilizing libraries such as NumPy and Matplotlib for effective data visualization. In Java, I have developed systems following the MVC pattern, focusing on CRUD operations and user management. Additionally, my expertise extends to C, where I have worked on embedded systems, emphasizing hardware-software integration and design._x000D_
+_x000D_
+Complementing my technical abilities are my soft skills, honed through collaborative teamwork and effective communication. I excel in active listening, critical thinking, and problem-solving, ensuring tasks are executed with precision and accuracy. My commitment to continuous improvement aligns with Mavericks' culture of learning and innovation._x000D_
+_x000D_
+I am excited about the opportunity to contribute to Mavericks Consulting and leverage my skills to drive impactful solutions. I am eager to undergo the application process outlined and am available at your earliest convenience for further discussions._x000D_
 _x000D_
 Best Regards,_x000D_
 Chuang Kai Siang</t>
   </si>
   <si>
-    <t>Subject: Application for Sales Engineer Position at Hermetic-Pumps Singapore_x000D_
+    <t>Subject: Application for Intern - Bids and Proposal Position_x000D_
 _x000D_
 Dear Hiring Manager,_x000D_
 _x000D_
-I hope this email finds you well. My name is Chuang Kai Siang, currently pursuing a Diploma in Computer Engineering at Temasek Polytechnic, now in my second year. I came across the Sales Engineer role at Hermetic-Pumps Singapore on Glints.com and was immediately drawn to the opportunity. My interest in this position stems from a strong desire to learn from experienced engineers and to follow in my father's footsteps, who holds a master's degree in engineering._x000D_
-_x000D_
-My technical skills, honed through my academic journey and practical projects, are well-aligned with the requirements of the Sales Engineer role. Proficient in Python, Java, and C, I have developed systems and implemented solutions that require a deep understanding of both hardware and software integration. Moreover, my experience in Python includes utilizing libraries like NumPy and Matplotlib for enhanced data visualization, while in Java, I've implemented CRUD systems following the MVC pattern. These technical competencies position me well to grasp the complexities of pump technology and effectively communicate their benefits to potential customers._x000D_
-_x000D_
-In addition to my technical proficiency, my soft skills further complement my suitability for this role. I excel in collaborative teamwork, leveraging strong active listening and interpersonal communication skills to foster productive working relationships. My ability to think critically and analytically enables me to solve problems efficiently and make informed decisions, ensuring tasks are completed with precision and accuracy. These skills are crucial in engaging with customers, understanding their fluid handling challenges, and providing tailored technical advice and solutions._x000D_
-_x000D_
-I am excited about the opportunity to contribute to Hermetic-Pumps Singapore and am confident that my blend of technical expertise and soft skills will enable me to excel in the Sales Engineer role. Thank you for considering my application. I look forward to the possibility of discussing how my background, skills, and motivations align with the needs of your team. _x000D_
+I am writing to express my interest in the Intern - Bids and Proposal position at Mgg Software Pte Ltd, as advertised on Glints.com. My name is Chuang Kai Siang, currently pursuing a Diploma in Computer Engineering at Temasek Polytechnic, Year 2. The opportunity to learn from experienced professionals aligns with my aspirations, particularly inspired by my father's engineering background._x000D_
+_x000D_
+My journey in discovering this role stems from a strong desire to broaden my skill set and delve into the intricacies of business strategies within a competitive environment. With a foundation in Python, Java, and C, I have honed my technical abilities, utilizing libraries like NumPy and Matplotlib for data visualization, implementing MVC patterns for system development, and integrating hardware and software in embedded systems._x000D_
+_x000D_
+Beyond technical proficiency, my experiences have cultivated soft skills crucial for collaborative environments. I excel in teamwork, leveraging active listening and interpersonal communication to foster productive relationships. My analytical prowess enables me to think critically, ensuring tasks are executed meticulously, meeting tight deadlines with precision._x000D_
+_x000D_
+Joining Mgg Software Pte Ltd as an Intern - Bids and Proposal presents an exciting opportunity to immerse myself in end-to-end tender activities, contributing to the company's success while furthering my professional growth. I am eager to apply my blend of technical expertise and soft skills to support the commercial team in identifying, vetting, and crafting compelling tender proposals._x000D_
+_x000D_
+Thank you for considering my application. I am enthusiastic about the prospect of contributing to Mgg Software Pte Ltd and am looking forward to the opportunity to discuss how my skills and experiences align with the company's vision._x000D_
 _x000D_
 Best Regards,_x000D_
 Chuang Kai Siang</t>
   </si>
   <si>
-    <t>Subject: Application for Mechanical Sales Engineer Position at Hermetic-Pumps Singapore_x000D_
+    <t>Subject: Application for Software Engineer Position at Monstyr Pte Ltd_x000D_
 _x000D_
 Dear Hiring Manager,_x000D_
 _x000D_
-I am writing to express my interest in the Mechanical Sales Engineer position at Hermetic-Pumps Singapore, as discovered on Glints.com. My name is Chuang Kai Siang, currently pursuing a Diploma in Computer Engineering at Temasek Polytechnic, Year 2. My aspiration to join your esteemed company stems from a strong desire to learn from experienced engineers, influenced by my father's footsteps, who holds a Master's in engineering._x000D_
-_x000D_
-Despite my background in computer engineering, my technical acumen extends beyond programming languages. Proficient in Python, Java, and C, I have leveraged my skills to develop systems ranging from data visualization to embedded systems integration. Moreover, my collaborative teamwork skills, honed through various projects, align seamlessly with the collaborative nature of the role, facilitating effective communication and problem-solving._x000D_
-_x000D_
-My exposure to Python has equipped me with data visualization capabilities using libraries such as NumPy and Matplotlib, while my Java proficiency extends to implementing CRUD systems following the MVC pattern. Additionally, my experience in C involves designing and integrating hardware and software for embedded systems, demonstrating adaptability and a keen analytical mindset crucial for addressing fluid handling challenges._x000D_
-_x000D_
-Beyond technical expertise, I bring to the table strong interpersonal communication skills, critical thinking abilities, and a meticulous approach to task completion. These soft skills, coupled with my technical proficiency, position me well to excel in creating effective sales strategies, communicating product benefits, and providing tailored solutions to customer needs._x000D_
-_x000D_
-In conclusion, I am enthusiastic about the opportunity to contribute to the success of Hermetic-Pumps Singapore as a Mechanical Sales Engineer. My blend of technical prowess and soft skills makes me a valuable asset to your team. Thank you for considering my application. I look forward to the possibility of discussing how I can contribute to your team further._x000D_
+I hope this email finds you well. My name is Chuang Kai Siang, and I am currently pursuing a Diploma in Computer Engineering at Temasek Polytechnic, now in my second year. I came across the Software Engineer position at Monstyr Pte Ltd on Glints.com, and I am writing to express my keen interest in joining your team._x000D_
+_x000D_
+My motivation for applying stems from a strong desire to learn from experienced engineers, coupled with a personal aspiration to follow in my father's footsteps, who holds a master's degree in engineering. My technical background includes proficiency in Python, where I've leveraged libraries like NumPy and Matplotlib for enhanced data visualization, as well as Java, where I've developed systems following the MVC pattern. Additionally, I have experience in C, particularly in embedded systems design and integration._x000D_
+_x000D_
+In terms of soft skills, I excel in collaborative teamwork, with a knack for active listening and effective interpersonal communication. I bring a critical and analytical thinking approach to problem-solving, ensuring tasks are completed with precision and accuracy. My goal is to contribute effectively to a dynamic team environment, leveraging both my technical expertise and soft skills to drive impactful outcomes._x000D_
+_x000D_
+I am excited about the opportunity to contribute to Monstyr's mission of creating O2O synergy through innovative solutions. The chance to work across the stack, from frontend to backend, on a public-facing web/mobile app aligns perfectly with my career aspirations. I am eager to tackle the challenges and learning opportunities that come with being part of a startup in its early stages, and I am committed to delivering high-quality results._x000D_
+_x000D_
+Thank you for considering my application. I am looking forward to the possibility of discussing how my skills and experiences align with the needs of your team further. Please find my expected salary indicated in my attached resume. _x000D_
 _x000D_
 Best Regards,_x000D_
 Chuang Kai Siang</t>
@@ -487,7 +489,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="171.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="168.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -495,12 +497,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
added a few changes
</commit_message>
<xml_diff>
--- a/InAuto_Project_2200589F_2202465G/InternshipEmails.xlsx
+++ b/InAuto_Project_2200589F_2202465G/InternshipEmails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78df99500250e0aa/Documents/GitHub/InAuto/InAuto_Project_2200589F_2202465G/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="198" documentId="8_{C36450E1-70C5-4284-8724-A0A78D84726F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4460674-0E73-4984-84EB-7E0BD29A0DD9}"/>
+  <xr:revisionPtr revIDLastSave="206" documentId="8_{C36450E1-70C5-4284-8724-A0A78D84726F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8303F5F6-A23D-4EE5-B80D-38E57858E74A}"/>
   <bookViews>
     <workbookView xWindow="5220" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{A8753D73-CDB8-4E0C-8DDE-BB08DD8360D8}"/>
   </bookViews>
@@ -41,89 +41,93 @@
     <t>Email Applications</t>
   </si>
   <si>
-    <t>Subject: Application for Front-End Developer/Software Intern Position at Aevice Health_x000D_
+    <t>Subject: Application for Front-End Developer Internship at Aevice Health_x000D_
 _x000D_
 Dear Hiring Manager,_x000D_
 _x000D_
-I am writing to express my interest in the Front-End Developer/Software Intern position at Aevice Health, as advertised on Glints.com. My name is Chuang Kai Siang, currently pursuing a Diploma in Computer Engineering at Temasek Polytechnic in my second year. I discovered this opportunity through Glints.com and was immediately drawn to Aevice Health due to its innovative approach to improving the lives of patients with chronic respiratory diseases, a cause close to my heart. Moreover, I am motivated to apply for this role as it aligns with my strong desire to learn from experienced engineers and follow in my father's footsteps, who holds a master's degree in engineering._x000D_
-_x000D_
-In terms of technical skills, I bring a robust foundation in programming languages such as Python, Java, and C. In Python, I have experience leveraging libraries like NumPy and Matplotlib for enhanced data visualization. My proficiency in Java extends to developing systems following the MVC pattern, implementing CRUD operations, and managing user interactions. Additionally, my expertise in C includes designing and integrating hardware and software for embedded systems. These technical skills position me well to contribute effectively to the development, testing, and maintenance of mobile and web applications at Aevice Health._x000D_
-_x000D_
-Complementing my technical abilities are my soft skills, which include a collaborative approach to teamwork, effective communication, and critical problem-solving. I excel in actively listening to team members' perspectives and offering valuable insights to drive project success. My ability to think critically and analytically ensures tasks are completed with precision and accuracy, contributing to a seamless development process. I am eager to further cultivate these skills within the dynamic environment at Aevice Health, where innovation and creativity are celebrated._x000D_
-_x000D_
-I am available for the flexible start/end dates specified in the job description and have included my GitHub profile in my application for your reference. I am excited about the opportunity to contribute to Aevice Health's mission and eager to gain hands-on experience in the software development lifecycle. Thank you for considering my application. _x000D_
+I hope this email finds you well. My name is Chuang Kai Siang, and I am currently a second-year student pursuing a Diploma in Computer Engineering at Temasek Polytechnic. I recently came across the Front-End Developer Internship opportunity at Aevice Health on Glints.com, and I am writing to express my strong interest in joining your team._x000D_
+_x000D_
+What drew me to Aevice Health is its commitment to innovation in healthcare technology, coupled with a culture that encourages creativity and ownership. As someone with a deep-rooted passion for learning and a desire to follow in my father's footsteps, who holds a master's in engineering, I am eager to contribute to Aevice Health's mission of improving the lives of patients with chronic respiratory diseases._x000D_
+_x000D_
+With a solid foundation in programming languages such as Python, Java, and C, I have experience in developing systems, implementing embedded systems, and utilizing libraries for data visualization. Moreover, my exposure to collaborative teamwork has honed my communication and problem-solving skills, ensuring tasks are completed with precision and efficiency._x000D_
+_x000D_
+I am particularly excited about the opportunity to translate UI/UX wireframes into front-end code, develop responsive web and mobile applications, and contribute to enhancing app usability through micro-interactions and animations. I am confident that my technical skills, coupled with my ability to work effectively in a team, make me a strong candidate for this role._x000D_
+_x000D_
+I am available for a flexible internship period from June to December 2024 and have included a link to my GitHub profile in my application. I am eager to gain hands-on experience in the full development lifecycle and further develop my skills in mobile application development._x000D_
+_x000D_
+Thank you for considering my application. I look forward to the opportunity to discuss how my skills and experiences align with the needs of Aevice Health. _x000D_
 _x000D_
 Best Regards,_x000D_
 Chuang Kai Siang</t>
   </si>
   <si>
-    <t>Subject: Application for Software Engineer - Remote Position_x000D_
+    <t>Subject: Application for Singapore - Senior Engineering Lead (Full-Remote) Position at Aha AI_x000D_
 _x000D_
 Dear Hiring Manager,_x000D_
 _x000D_
-I hope this email finds you well. My name is Chuang Kai Siang, and I am writing to express my interest in the Software Engineer position at Kopi Date, as advertised on Glints.com. As a second-year student pursuing a Diploma in Computer Engineering at Temasek Polytechnic, I am deeply motivated to learn from experienced engineers and continue the legacy set by my father, who holds a master's degree in engineering._x000D_
-_x000D_
-My journey into the world of programming began with Python, where I gained proficiency in utilizing libraries such as NumPy and Matplotlib for advanced data visualization. Additionally, my experience with Java involved developing systems following the MVC pattern, focusing on CRUD operations and user management. Furthermore, I have a solid foundation in C, particularly in implementing embedded systems that integrate hardware and software seamlessly._x000D_
-_x000D_
-Beyond technical expertise, I bring a set of soft skills that complement my technical capabilities. I excel in collaborative teamwork, leveraging strong active listening and interpersonal communication skills to foster a cohesive work environment. My ability to think critically and analytically enables me to solve problems effectively, ensuring tasks are completed with precision and accuracy._x000D_
-_x000D_
-I am particularly drawn to Kopi Date's commitment to developing user features, optimizing operations, and enhancing machine learning algorithms. My skills in JavaScript, Node.js, and Firebase align well with the role's requirements, and I am eager to contribute to the development of innovative solutions while continuously learning and growing within your dynamic team._x000D_
-_x000D_
-Thank you for considering my application. I am enthusiastic about the opportunity to further discuss how my skills and experiences align with the needs of Kopi Date. Please find my attached resume for more details. _x000D_
+I am writing to express my interest in the Singapore - Senior Engineering Lead (Full-Remote) position at Aha AI, as found on Glints.com. My name is Chuang Kai Siang, currently pursuing a Diploma in Computer Engineering at Temasek Polytechnic in my second year. My passion for engineering stems from my father's influence, who holds a master's degree in engineering, igniting in me a strong desire to learn from experienced professionals in the field._x000D_
+_x000D_
+With a solid foundation in technical skills, I bring proficiency in Python, leveraging libraries like NumPy and Matplotlib for data visualization, Java for developing systems adhering to the MVC pattern, and C for embedded systems integration. Moreover, my collaborative nature and adeptness in active listening and communication complement my technical acumen, ensuring seamless teamwork and problem-solving._x000D_
+_x000D_
+My experience in collaborative teamwork, combined with critical thinking and analytical prowess, equips me to contribute effectively to Aha AI's innovative projects. I am committed to delivering tasks with precision and accuracy, aligning with Aha AI's culture of practicality and creativity._x000D_
+_x000D_
+Thank you for considering my application. I am eager to bring my skills and enthusiasm to Aha AI's dynamic team. _x000D_
 _x000D_
 Best Regards,_x000D_
 Chuang Kai Siang</t>
   </si>
   <si>
-    <t>Subject: Application for Junior Software Developer Position at Mavericks Consulting_x000D_
+    <t>Subject: Application for Remote Software Engineer Role at Atomionics_x000D_
 _x000D_
 Dear Hiring Manager,_x000D_
 _x000D_
-I hope this email finds you well. I am writing to express my keen interest in the Junior Software Developer position at Mavericks Consulting, as advertised on Glints.com. My name is Chuang Kai Siang, currently pursuing a Diploma in Computer Engineering at Temasek Polytechnic, Singapore, in my second year._x000D_
-_x000D_
-My journey into the world of software development has been inspired by my father, who holds a master's degree in engineering. I am eager to follow in his footsteps and learn from experienced engineers like those at Mavericks Consulting. My main motivation for applying is to immerse myself in a dynamic environment where I can continuously grow and contribute to meaningful projects._x000D_
-_x000D_
-With a solid foundation in technical skills, I have hands-on experience in Python, utilizing libraries such as NumPy and Matplotlib for effective data visualization. In Java, I have developed systems following the MVC pattern, focusing on CRUD operations and user management. Additionally, my expertise extends to C, where I have worked on embedded systems, emphasizing hardware-software integration and design._x000D_
-_x000D_
-Complementing my technical abilities are my soft skills, honed through collaborative teamwork and effective communication. I excel in active listening, critical thinking, and problem-solving, ensuring tasks are executed with precision and accuracy. My commitment to continuous improvement aligns with Mavericks' culture of learning and innovation._x000D_
-_x000D_
-I am excited about the opportunity to contribute to Mavericks Consulting and leverage my skills to drive impactful solutions. I am eager to undergo the application process outlined and am available at your earliest convenience for further discussions._x000D_
+I hope this email finds you well. My name is Chuang Kai Siang, currently pursuing a Diploma in Computer Engineering at Temasek Polytechnic, Year 2. I recently came across the opportunity for the Remote Software Engineer position at Atomionics through Glints.com, and I am writing to express my strong interest in the role._x000D_
+_x000D_
+What particularly excites me about this position is the opportunity to learn from experienced engineers and contribute to cutting-edge technology, especially in the realm of quantum sensors. My passion for software engineering stems from a desire to follow in my father's footsteps, who has his masters in engineering, and I am eager to immerse myself in a dynamic environment where innovation thrives._x000D_
+_x000D_
+With a solid foundation in Python, Java, and C programming languages, I have honed my skills through hands-on projects. In Python, I have experience importing libraries like NumPy and Matplotlib for advanced data visualization, while in Java, I have developed systems following the MVC pattern. Additionally, my proficiency in C extends to embedded systems, focusing on hardware-software integration._x000D_
+_x000D_
+Beyond technical expertise, I bring to the table strong collaborative teamwork skills, coupled with active listening and effective communication abilities. I approach problem-solving with a critical and analytical mindset, ensuring tasks are completed with precision and efficiency._x000D_
+_x000D_
+I am eager to contribute my skills to Atomionics, where I see an opportunity to learn and grow while making meaningful contributions to the advancement of quantum technology. I am confident that my technical proficiency and soft skills make me a strong fit for this role._x000D_
+_x000D_
+Thank you for considering my application. I am looking forward to the possibility of discussing how I can contribute to Atomionics further._x000D_
 _x000D_
 Best Regards,_x000D_
 Chuang Kai Siang</t>
   </si>
   <si>
-    <t>Subject: Application for Intern - Bids and Proposal Position_x000D_
+    <t>Subject: Application for Electronics Engineering Internship Position at Atomionics_x000D_
 _x000D_
 Dear Hiring Manager,_x000D_
 _x000D_
-I am writing to express my interest in the Intern - Bids and Proposal position at Mgg Software Pte Ltd, as advertised on Glints.com. My name is Chuang Kai Siang, currently pursuing a Diploma in Computer Engineering at Temasek Polytechnic, Year 2. The opportunity to learn from experienced professionals aligns with my aspirations, particularly inspired by my father's engineering background._x000D_
-_x000D_
-My journey in discovering this role stems from a strong desire to broaden my skill set and delve into the intricacies of business strategies within a competitive environment. With a foundation in Python, Java, and C, I have honed my technical abilities, utilizing libraries like NumPy and Matplotlib for data visualization, implementing MVC patterns for system development, and integrating hardware and software in embedded systems._x000D_
-_x000D_
-Beyond technical proficiency, my experiences have cultivated soft skills crucial for collaborative environments. I excel in teamwork, leveraging active listening and interpersonal communication to foster productive relationships. My analytical prowess enables me to think critically, ensuring tasks are executed meticulously, meeting tight deadlines with precision._x000D_
-_x000D_
-Joining Mgg Software Pte Ltd as an Intern - Bids and Proposal presents an exciting opportunity to immerse myself in end-to-end tender activities, contributing to the company's success while furthering my professional growth. I am eager to apply my blend of technical expertise and soft skills to support the commercial team in identifying, vetting, and crafting compelling tender proposals._x000D_
-_x000D_
-Thank you for considering my application. I am enthusiastic about the prospect of contributing to Mgg Software Pte Ltd and am looking forward to the opportunity to discuss how my skills and experiences align with the company's vision._x000D_
+I hope this email finds you well. I am writing to express my keen interest in the Electronics Engineering Internship position at Atomionics, as advertised on Glints.com. My name is Chuang Kai Siang, currently pursuing a Diploma in Computer Engineering at Temasek Polytechnic, in my second year of study._x000D_
+_x000D_
+My fascination with electronics and a strong desire to learn from experienced engineers, coupled with a personal connection to the field through my father, who holds a Master's in Engineering, motivates my application for this role. The opportunity to contribute to cutting-edge research and product development in a high-growth startup like Atomionics is incredibly exciting to me._x000D_
+_x000D_
+In terms of technical skills, I bring a robust foundation in Python, utilizing libraries such as NumPy and Matplotlib for advanced data visualization. Additionally, my proficiency in Java includes developing systems following the MVC pattern, emphasizing CRUD operations and user management. Furthermore, my experience in C has equipped me with the ability to implement embedded systems, focusing on the seamless integration of hardware and software components._x000D_
+_x000D_
+Complementing my technical abilities are my soft skills, including collaborative teamwork, active listening, and strong interpersonal communication. I excel in critical thinking and problem-solving, ensuring tasks are completed with precision and efficiency. My commitment to accuracy and attention to detail enables me to tackle challenges effectively, contributing positively to team dynamics._x000D_
+_x000D_
+I am enthusiastic about the prospect of working with Atomionics to gain valuable insights into deep tech research and product development within the quantum technology space. I am eager to leverage my skills and contribute meaningfully to your team. Thank you for considering my application._x000D_
 _x000D_
 Best Regards,_x000D_
 Chuang Kai Siang</t>
   </si>
   <si>
-    <t>Subject: Application for Software Engineer Position at Monstyr Pte Ltd_x000D_
+    <t>Subject: Application for Software Engineering (Python) Internship at Atomionics_x000D_
 _x000D_
 Dear Hiring Manager,_x000D_
 _x000D_
-I hope this email finds you well. My name is Chuang Kai Siang, and I am currently pursuing a Diploma in Computer Engineering at Temasek Polytechnic, now in my second year. I came across the Software Engineer position at Monstyr Pte Ltd on Glints.com, and I am writing to express my keen interest in joining your team._x000D_
-_x000D_
-My motivation for applying stems from a strong desire to learn from experienced engineers, coupled with a personal aspiration to follow in my father's footsteps, who holds a master's degree in engineering. My technical background includes proficiency in Python, where I've leveraged libraries like NumPy and Matplotlib for enhanced data visualization, as well as Java, where I've developed systems following the MVC pattern. Additionally, I have experience in C, particularly in embedded systems design and integration._x000D_
-_x000D_
-In terms of soft skills, I excel in collaborative teamwork, with a knack for active listening and effective interpersonal communication. I bring a critical and analytical thinking approach to problem-solving, ensuring tasks are completed with precision and accuracy. My goal is to contribute effectively to a dynamic team environment, leveraging both my technical expertise and soft skills to drive impactful outcomes._x000D_
-_x000D_
-I am excited about the opportunity to contribute to Monstyr's mission of creating O2O synergy through innovative solutions. The chance to work across the stack, from frontend to backend, on a public-facing web/mobile app aligns perfectly with my career aspirations. I am eager to tackle the challenges and learning opportunities that come with being part of a startup in its early stages, and I am committed to delivering high-quality results._x000D_
-_x000D_
-Thank you for considering my application. I am looking forward to the possibility of discussing how my skills and experiences align with the needs of your team further. Please find my expected salary indicated in my attached resume. _x000D_
+I hope this email finds you well. My name is Chuang Kai Siang, and I am currently pursuing a Diploma in Computer Engineering at Temasek Polytechnic, in my second year. I recently came across the opportunity for the Software Engineering (Python) Internship at Atomionics through Glints.com. What attracted me most to this role is not only my strong desire to learn from experienced engineers but also the opportunity to follow in my father's footsteps, who holds a master's in engineering._x000D_
+_x000D_
+My technical background includes proficient skills in Python, where I have experience in utilizing libraries such as NumPy and Matplotlib for enhanced data visualization. Additionally, I am skilled in Java, having developed systems following the MVC pattern, and proficient in C for embedded systems design and integration. My exposure to electro-mechanical functionalities and data gathering aligns well with the responsibilities of the front-end and back-end aspects of the role at Atomionics._x000D_
+_x000D_
+In terms of soft skills, I excel in collaborative teamwork, actively listening to others' perspectives while effectively communicating my own. I possess strong critical thinking abilities, enabling me to solve problems analytically and make well-informed decisions. With a keen eye for detail, I ensure tasks are completed accurately and efficiently, contributing to overall project success._x000D_
+_x000D_
+I am genuinely excited about the opportunity to contribute to Atomionics and further develop my skills in software engineering within the realm of quantum technology. The chance to work on cutting-edge projects and learn from a dynamic team is something I am eager to embrace. I am confident that my technical expertise and soft skills make me a strong fit for this role._x000D_
+_x000D_
+Thank you for considering my application. I look forward to the possibility of discussing how I can contribute to Atomionics further. _x000D_
 _x000D_
 Best Regards,_x000D_
 Chuang Kai Siang</t>
@@ -489,7 +493,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="168.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="168" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -497,17 +501,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="360" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -517,7 +521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>